<commit_message>
added poamoho gage, RF thresholds, and min + max values for all gauge charts
</commit_message>
<xml_diff>
--- a/BRIAN/Min_Max_Gauge_Data/Min_Max_Gauges.xlsx
+++ b/BRIAN/Min_Max_Gauge_Data/Min_Max_Gauges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgorb\OneDrive\Documents\GitHub\Windward_Oahu_Flooding_App_resources\BRIAN\Min_Max_Gauge_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64399A81-C1C9-48E7-A918-D9BE1686FE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741EE35A-9CFF-4143-91BD-3F492B61A34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12960" yWindow="1530" windowWidth="14310" windowHeight="14205" xr2:uid="{863069AA-8057-459F-BC1E-F50BB452D23B}"/>
+    <workbookView xWindow="13755" yWindow="2145" windowWidth="14310" windowHeight="14205" xr2:uid="{863069AA-8057-459F-BC1E-F50BB452D23B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Gauge</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Min_val</t>
+  </si>
+  <si>
+    <t>Poamoho rain</t>
   </si>
 </sst>
 </file>
@@ -409,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{466CF2B3-D8DE-4A5E-92CE-E1BB4B368D5C}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,6 +478,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>